<commit_message>
Stories / TPS update
Added abstract and product description to Stories
</commit_message>
<xml_diff>
--- a/docs/TPS Screen Project.xlsx
+++ b/docs/TPS Screen Project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jonah/Documents/TouchscreenInterface/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462456F9-138C-C948-9231-4A2E8283EF08}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D44D30-B9FC-0A4B-B6F4-DF576F87D022}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="920" yWindow="460" windowWidth="24680" windowHeight="15540" tabRatio="985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="85">
   <si>
     <t>Date: 04/21/2018</t>
   </si>
@@ -280,6 +280,9 @@
   </si>
   <si>
     <t>Date: 10/06/2018</t>
+  </si>
+  <si>
+    <t>Add the option to run a video in the ads section.  Possibly mp3</t>
   </si>
 </sst>
 </file>
@@ -379,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -409,6 +412,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -791,10 +795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I263"/>
+  <dimension ref="A1:I264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A229" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A249" sqref="A249"/>
+    <sheetView tabSelected="1" topLeftCell="A232" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A264" sqref="A264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4049,8 +4053,28 @@
         <v>59</v>
       </c>
     </row>
+    <row r="264" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A264" s="19" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="A23:G23"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="A43:G43"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="A51:G51"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="A59:G59"/>
+    <mergeCell ref="E65:G65"/>
     <mergeCell ref="E90:G90"/>
     <mergeCell ref="A92:G92"/>
     <mergeCell ref="A67:G67"/>
@@ -4058,21 +4082,6 @@
     <mergeCell ref="A75:G75"/>
     <mergeCell ref="E81:G81"/>
     <mergeCell ref="A83:G83"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="A51:G51"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="A59:G59"/>
-    <mergeCell ref="E65:G65"/>
-    <mergeCell ref="A23:G23"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="A43:G43"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="A13:G13"/>
-    <mergeCell ref="E21:G21"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Added notes to tps
</commit_message>
<xml_diff>
--- a/docs/TPS Screen Project.xlsx
+++ b/docs/TPS Screen Project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jonah/Documents/TouchscreenInterface/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DD061F-647C-D447-8E31-4E3BB10359FE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FFADCB5-5048-E54C-9A15-DE26D8761EC2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="920" yWindow="460" windowWidth="24680" windowHeight="15540" tabRatio="985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="104">
   <si>
     <t>Date: 04/21/2018</t>
   </si>
@@ -334,6 +334,12 @@
   </si>
   <si>
     <t>Met again with the client.  He has requested that we set up another USB drive.</t>
+  </si>
+  <si>
+    <t>Updates: set_xinput_matrix.sh fails when Touch Screen is not found</t>
+  </si>
+  <si>
+    <t>setWindowSizes.sh failed</t>
   </si>
 </sst>
 </file>
@@ -849,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I294"/>
+  <dimension ref="A1:I297"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A277" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A290" sqref="A290:A294"/>
+      <selection activeCell="A290" sqref="A290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4506,48 +4512,43 @@
         <v>14</v>
       </c>
     </row>
+    <row r="289" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A289" s="18" t="s">
+        <v>102</v>
+      </c>
+    </row>
     <row r="290" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A290" s="15" t="s">
+      <c r="A290" s="18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A293" s="15" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="291" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A291" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="292" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A292" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="293" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A293" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="294" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A295" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A296" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A297" s="1" t="s">
         <v>100</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="A13:G13"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="A23:G23"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="A43:G43"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="A51:G51"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="A59:G59"/>
-    <mergeCell ref="E65:G65"/>
     <mergeCell ref="E90:G90"/>
     <mergeCell ref="A92:G92"/>
     <mergeCell ref="A67:G67"/>
@@ -4555,6 +4556,21 @@
     <mergeCell ref="A75:G75"/>
     <mergeCell ref="E81:G81"/>
     <mergeCell ref="A83:G83"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="A51:G51"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="A59:G59"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="A23:G23"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="A43:G43"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="E21:G21"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>